<commit_message>
updated comparison table and checked all missing values
</commit_message>
<xml_diff>
--- a/summaries/comparison_excel.xlsx
+++ b/summaries/comparison_excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewjohnston/coding_projects/complete_reproduction_folder/summaries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCB03736-DE87-784C-8613-3C31C5C6121B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AD01765-0D04-2F40-966C-5B8B7A65C710}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19200" yWindow="500" windowWidth="19200" windowHeight="20020" xr2:uid="{8AEC59CE-BB56-A04F-9F36-173874C2CDE5}"/>
   </bookViews>
@@ -542,11 +542,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E46FF3E9-1C3A-0442-9272-FBA04DEE03AE}">
   <dimension ref="A1:O34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="J3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="L11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="O32" sqref="O32"/>
+      <selection pane="bottomRight" activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -985,7 +985,7 @@
       <c r="B20">
         <v>-0.497</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="7">
         <v>6.5446999999999996E-3</v>
       </c>
       <c r="D20">
@@ -1145,7 +1145,7 @@
       <c r="B24">
         <v>52.603000000000002</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="7">
         <v>0.55505110000000002</v>
       </c>
       <c r="D24" s="5">
@@ -1225,7 +1225,7 @@
       <c r="B26">
         <v>16.684000000000001</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="7">
         <v>0.24619550000000001</v>
       </c>
       <c r="D26">
@@ -1281,7 +1281,7 @@
       <c r="B28">
         <v>-30.457999999999998</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="7">
         <v>-0.46680329999999998</v>
       </c>
       <c r="D28">
@@ -1401,7 +1401,7 @@
       <c r="B32">
         <v>61.62</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="7">
         <v>71.81</v>
       </c>
       <c r="D32">

</xml_diff>